<commit_message>
Ajustes para entrega + modelos
</commit_message>
<xml_diff>
--- a/MP4/Validation_results.xlsx
+++ b/MP4/Validation_results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Projects\Imagenes\Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danie\Documents\Projects\Imagenes\Laboratorio\MP4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3467E2C2-F341-4981-B672-1B09EFEF38A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E993CA88-F146-4B42-8893-DD6D3EF623CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13425" activeTab="3" xr2:uid="{6EA93847-BA76-4D2A-B05E-09FBFE9B4B89}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="17">
   <si>
     <t>Histogram Function</t>
   </si>
@@ -86,6 +86,9 @@
   </si>
   <si>
     <t>Max</t>
+  </si>
+  <si>
+    <t>RGB2LAB</t>
   </si>
 </sst>
 </file>
@@ -176,14 +179,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6369,69 +6372,69 @@
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -6469,7 +6472,7 @@
       </c>
     </row>
     <row r="9" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -6505,7 +6508,7 @@
       </c>
     </row>
     <row r="10" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -6544,7 +6547,7 @@
       </c>
     </row>
     <row r="11" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -6580,7 +6583,7 @@
       </c>
     </row>
     <row r="12" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -6616,7 +6619,7 @@
       </c>
     </row>
     <row r="13" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5">
         <v>7</v>
       </c>
@@ -6652,7 +6655,7 @@
       </c>
     </row>
     <row r="14" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5">
         <v>9</v>
       </c>
@@ -6688,7 +6691,7 @@
       </c>
     </row>
     <row r="15" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5">
         <v>10</v>
       </c>
@@ -6724,7 +6727,7 @@
       </c>
     </row>
     <row r="16" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5">
         <v>15</v>
       </c>
@@ -6760,7 +6763,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5">
         <v>20</v>
       </c>
@@ -6796,7 +6799,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -6834,7 +6837,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="5">
         <v>2</v>
       </c>
@@ -6870,7 +6873,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5">
         <v>3</v>
       </c>
@@ -6906,7 +6909,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5">
         <v>4</v>
       </c>
@@ -6942,7 +6945,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5">
         <v>5</v>
       </c>
@@ -6978,7 +6981,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -7014,7 +7017,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5">
         <v>9</v>
       </c>
@@ -7050,7 +7053,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="5">
         <v>10</v>
       </c>
@@ -7086,7 +7089,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="5">
         <v>15</v>
       </c>
@@ -7122,7 +7125,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="5">
         <v>20</v>
       </c>
@@ -7158,7 +7161,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -7196,7 +7199,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="5">
         <v>2</v>
       </c>
@@ -7232,7 +7235,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="5">
         <v>3</v>
       </c>
@@ -7268,7 +7271,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="5">
         <v>4</v>
       </c>
@@ -7304,7 +7307,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" s="11"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="5">
         <v>5</v>
       </c>
@@ -7340,7 +7343,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="5">
         <v>7</v>
       </c>
@@ -7376,7 +7379,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="5">
         <v>9</v>
       </c>
@@ -7412,7 +7415,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="5">
         <v>10</v>
       </c>
@@ -7448,7 +7451,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="5">
         <v>15</v>
       </c>
@@ -7484,7 +7487,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="5">
         <v>20</v>
       </c>
@@ -7523,7 +7526,7 @@
       <c r="B42" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="11">
         <f>AVERAGE(C31:L39)</f>
         <v>0.23058888888888901</v>
       </c>
@@ -7532,7 +7535,7 @@
       <c r="B43" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="11">
         <f>_xlfn.STDEV.P(C31:L39)</f>
         <v>8.6921662616972317E-2</v>
       </c>
@@ -7589,69 +7592,69 @@
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -7689,7 +7692,7 @@
       </c>
     </row>
     <row r="9" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -7725,7 +7728,7 @@
       </c>
     </row>
     <row r="10" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -7764,7 +7767,7 @@
       </c>
     </row>
     <row r="11" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -7800,7 +7803,7 @@
       </c>
     </row>
     <row r="12" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -7836,7 +7839,7 @@
       </c>
     </row>
     <row r="13" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5">
         <v>7</v>
       </c>
@@ -7872,7 +7875,7 @@
       </c>
     </row>
     <row r="14" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5">
         <v>9</v>
       </c>
@@ -7908,7 +7911,7 @@
       </c>
     </row>
     <row r="15" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5">
         <v>10</v>
       </c>
@@ -7944,7 +7947,7 @@
       </c>
     </row>
     <row r="16" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5">
         <v>15</v>
       </c>
@@ -7980,7 +7983,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5">
         <v>20</v>
       </c>
@@ -8016,7 +8019,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -8054,7 +8057,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="5">
         <v>2</v>
       </c>
@@ -8100,7 +8103,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5">
         <v>3</v>
       </c>
@@ -8146,7 +8149,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5">
         <v>4</v>
       </c>
@@ -8192,7 +8195,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5">
         <v>5</v>
       </c>
@@ -8238,7 +8241,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -8284,7 +8287,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5">
         <v>9</v>
       </c>
@@ -8330,7 +8333,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="5">
         <v>10</v>
       </c>
@@ -8376,7 +8379,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="5">
         <v>15</v>
       </c>
@@ -8422,7 +8425,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="5">
         <v>20</v>
       </c>
@@ -8468,7 +8471,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -8506,7 +8509,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="5">
         <v>2</v>
       </c>
@@ -8552,7 +8555,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="5">
         <v>3</v>
       </c>
@@ -8598,7 +8601,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="5">
         <v>4</v>
       </c>
@@ -8644,7 +8647,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" s="11"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="5">
         <v>5</v>
       </c>
@@ -8690,7 +8693,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="5">
         <v>7</v>
       </c>
@@ -8736,7 +8739,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="5">
         <v>9</v>
       </c>
@@ -8782,7 +8785,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="5">
         <v>10</v>
       </c>
@@ -8828,7 +8831,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="5">
         <v>15</v>
       </c>
@@ -8874,7 +8877,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="5">
         <v>20</v>
       </c>
@@ -8923,7 +8926,7 @@
       <c r="B42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="11">
         <f>AVERAGE(C31:L39)</f>
         <v>0.27033333333333343</v>
       </c>
@@ -8932,7 +8935,7 @@
       <c r="B43" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="11">
         <f>_xlfn.STDEV.P(C31:L39)</f>
         <v>9.8046814215341963E-2</v>
       </c>
@@ -8975,7 +8978,7 @@
   <dimension ref="A4:XFD45"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+      <selection activeCell="C7" sqref="C7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.45"/>
@@ -8989,69 +8992,69 @@
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="C6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -9089,7 +9092,7 @@
       </c>
     </row>
     <row r="9" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -9125,7 +9128,7 @@
       </c>
     </row>
     <row r="10" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -9164,7 +9167,7 @@
       </c>
     </row>
     <row r="11" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -9200,7 +9203,7 @@
       </c>
     </row>
     <row r="12" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -9236,7 +9239,7 @@
       </c>
     </row>
     <row r="13" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5">
         <v>7</v>
       </c>
@@ -9272,7 +9275,7 @@
       </c>
     </row>
     <row r="14" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5">
         <v>9</v>
       </c>
@@ -9308,7 +9311,7 @@
       </c>
     </row>
     <row r="15" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5">
         <v>10</v>
       </c>
@@ -9344,7 +9347,7 @@
       </c>
     </row>
     <row r="16" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5">
         <v>15</v>
       </c>
@@ -9380,7 +9383,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5">
         <v>20</v>
       </c>
@@ -9416,7 +9419,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -9454,7 +9457,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="5">
         <v>2</v>
       </c>
@@ -9500,7 +9503,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5">
         <v>3</v>
       </c>
@@ -9546,7 +9549,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5">
         <v>4</v>
       </c>
@@ -9592,7 +9595,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5">
         <v>5</v>
       </c>
@@ -9638,7 +9641,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -9684,7 +9687,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5">
         <v>9</v>
       </c>
@@ -9730,7 +9733,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="5">
         <v>10</v>
       </c>
@@ -9776,7 +9779,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="5">
         <v>15</v>
       </c>
@@ -9822,7 +9825,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="5">
         <v>20</v>
       </c>
@@ -9868,7 +9871,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -9906,7 +9909,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="5">
         <v>2</v>
       </c>
@@ -9952,7 +9955,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="5">
         <v>3</v>
       </c>
@@ -9998,7 +10001,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="5">
         <v>4</v>
       </c>
@@ -10044,7 +10047,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" s="11"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="5">
         <v>5</v>
       </c>
@@ -10090,7 +10093,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="5">
         <v>7</v>
       </c>
@@ -10136,7 +10139,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="5">
         <v>9</v>
       </c>
@@ -10182,7 +10185,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="5">
         <v>10</v>
       </c>
@@ -10228,7 +10231,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="5">
         <v>15</v>
       </c>
@@ -10274,7 +10277,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="5">
         <v>20</v>
       </c>
@@ -10323,7 +10326,7 @@
       <c r="B42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="11">
         <f>AVERAGE(C31:L39)</f>
         <v>0.20836666666666684</v>
       </c>
@@ -10332,7 +10335,7 @@
       <c r="B43" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="11">
         <f>_xlfn.STDEV.P(C31:L39)</f>
         <v>7.5747746574476207E-2</v>
       </c>
@@ -10375,7 +10378,7 @@
   <dimension ref="A4:XFD45"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42:C45"/>
+      <selection activeCell="C7" sqref="C7:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.4" x14ac:dyDescent="0.45"/>
@@ -10389,69 +10392,69 @@
         <v>0</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="12"/>
-      <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="13"/>
+      <c r="G4" s="13"/>
+      <c r="H4" s="13"/>
+      <c r="I4" s="13"/>
+      <c r="J4" s="13"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
     </row>
     <row r="5" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
+      <c r="D5" s="13"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="13"/>
+      <c r="J5" s="13"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
     </row>
     <row r="6" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
+      <c r="C6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13"/>
     </row>
     <row r="7" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="13"/>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -10489,7 +10492,7 @@
       </c>
     </row>
     <row r="9" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A9" s="11"/>
+      <c r="A9" s="12"/>
       <c r="B9" s="5">
         <v>2</v>
       </c>
@@ -10525,7 +10528,7 @@
       </c>
     </row>
     <row r="10" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A10" s="11"/>
+      <c r="A10" s="12"/>
       <c r="B10" s="5">
         <v>3</v>
       </c>
@@ -10564,7 +10567,7 @@
       </c>
     </row>
     <row r="11" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A11" s="11"/>
+      <c r="A11" s="12"/>
       <c r="B11" s="5">
         <v>4</v>
       </c>
@@ -10600,7 +10603,7 @@
       </c>
     </row>
     <row r="12" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A12" s="11"/>
+      <c r="A12" s="12"/>
       <c r="B12" s="5">
         <v>5</v>
       </c>
@@ -10636,7 +10639,7 @@
       </c>
     </row>
     <row r="13" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A13" s="11"/>
+      <c r="A13" s="12"/>
       <c r="B13" s="5">
         <v>7</v>
       </c>
@@ -10672,7 +10675,7 @@
       </c>
     </row>
     <row r="14" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A14" s="11"/>
+      <c r="A14" s="12"/>
       <c r="B14" s="5">
         <v>9</v>
       </c>
@@ -10708,7 +10711,7 @@
       </c>
     </row>
     <row r="15" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A15" s="11"/>
+      <c r="A15" s="12"/>
       <c r="B15" s="5">
         <v>10</v>
       </c>
@@ -10744,7 +10747,7 @@
       </c>
     </row>
     <row r="16" spans="1:12 16384:16384" x14ac:dyDescent="0.45">
-      <c r="A16" s="11"/>
+      <c r="A16" s="12"/>
       <c r="B16" s="5">
         <v>15</v>
       </c>
@@ -10780,7 +10783,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A17" s="11"/>
+      <c r="A17" s="12"/>
       <c r="B17" s="5">
         <v>20</v>
       </c>
@@ -10816,7 +10819,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>6</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -10854,7 +10857,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A20" s="11"/>
+      <c r="A20" s="12"/>
       <c r="B20" s="5">
         <v>2</v>
       </c>
@@ -10900,7 +10903,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A21" s="11"/>
+      <c r="A21" s="12"/>
       <c r="B21" s="5">
         <v>3</v>
       </c>
@@ -10946,7 +10949,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A22" s="11"/>
+      <c r="A22" s="12"/>
       <c r="B22" s="5">
         <v>4</v>
       </c>
@@ -10992,7 +10995,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A23" s="11"/>
+      <c r="A23" s="12"/>
       <c r="B23" s="5">
         <v>5</v>
       </c>
@@ -11038,7 +11041,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A24" s="11"/>
+      <c r="A24" s="12"/>
       <c r="B24" s="5">
         <v>7</v>
       </c>
@@ -11084,7 +11087,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A25" s="11"/>
+      <c r="A25" s="12"/>
       <c r="B25" s="5">
         <v>9</v>
       </c>
@@ -11130,7 +11133,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A26" s="11"/>
+      <c r="A26" s="12"/>
       <c r="B26" s="5">
         <v>10</v>
       </c>
@@ -11176,7 +11179,7 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="11"/>
+      <c r="A27" s="12"/>
       <c r="B27" s="5">
         <v>15</v>
       </c>
@@ -11222,7 +11225,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A28" s="11"/>
+      <c r="A28" s="12"/>
       <c r="B28" s="5">
         <v>20</v>
       </c>
@@ -11268,7 +11271,7 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A30" s="11" t="s">
+      <c r="A30" s="12" t="s">
         <v>7</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -11306,7 +11309,7 @@
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A31" s="11"/>
+      <c r="A31" s="12"/>
       <c r="B31" s="5">
         <v>2</v>
       </c>
@@ -11352,7 +11355,7 @@
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A32" s="11"/>
+      <c r="A32" s="12"/>
       <c r="B32" s="5">
         <v>3</v>
       </c>
@@ -11398,7 +11401,7 @@
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A33" s="11"/>
+      <c r="A33" s="12"/>
       <c r="B33" s="5">
         <v>4</v>
       </c>
@@ -11444,7 +11447,7 @@
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A34" s="11"/>
+      <c r="A34" s="12"/>
       <c r="B34" s="5">
         <v>5</v>
       </c>
@@ -11490,7 +11493,7 @@
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A35" s="11"/>
+      <c r="A35" s="12"/>
       <c r="B35" s="5">
         <v>7</v>
       </c>
@@ -11536,7 +11539,7 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="5">
         <v>9</v>
       </c>
@@ -11582,7 +11585,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="5">
         <v>10</v>
       </c>
@@ -11628,7 +11631,7 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="5">
         <v>15</v>
       </c>
@@ -11674,7 +11677,7 @@
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A39" s="11"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="5">
         <v>20</v>
       </c>
@@ -11723,7 +11726,7 @@
       <c r="B42" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C42" s="13">
+      <c r="C42" s="11">
         <f>AVERAGE(C31:L39)</f>
         <v>0.19932222222222234</v>
       </c>
@@ -11732,7 +11735,7 @@
       <c r="B43" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="13">
+      <c r="C43" s="11">
         <f>_xlfn.STDEV.P(C31:L39)</f>
         <v>0.11787166540849775</v>
       </c>

</xml_diff>